<commit_message>
form A e form B
</commit_message>
<xml_diff>
--- a/analise_engajamento.xlsx
+++ b/analise_engajamento.xlsx
@@ -70,8 +70,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00006400"/>
-        <bgColor rgb="00006400"/>
+        <fgColor rgb="00FFC107"/>
+        <bgColor rgb="00FFC107"/>
       </patternFill>
     </fill>
     <fill>
@@ -82,8 +82,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFC107"/>
-        <bgColor rgb="00FFC107"/>
+        <fgColor rgb="00006400"/>
+        <bgColor rgb="00006400"/>
       </patternFill>
     </fill>
     <fill>
@@ -591,7 +591,7 @@
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Form 4 2025
-(Esperado: 7)</t>
+(Esperado: 8)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -637,7 +637,7 @@
       </c>
       <c r="I2" s="6" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
       </c>
       <c r="I4" s="6" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
     </row>
@@ -758,7 +758,7 @@
       <c r="H5" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I5" s="8" t="inlineStr">
+      <c r="I5" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -799,7 +799,7 @@
       <c r="H6" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I6" s="8" t="inlineStr">
+      <c r="I6" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -924,7 +924,7 @@
       </c>
       <c r="I9" s="6" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
     </row>
@@ -963,7 +963,7 @@
       <c r="H10" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I10" s="6" t="inlineStr">
+      <c r="I10" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1004,7 +1004,7 @@
       <c r="H11" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I11" s="6" t="inlineStr">
+      <c r="I11" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1043,9 +1043,9 @@
         <v>1</v>
       </c>
       <c r="H12" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="I12" s="8" t="inlineStr">
+        <v>7</v>
+      </c>
+      <c r="I12" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1086,7 +1086,7 @@
       <c r="H13" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I13" s="6" t="inlineStr">
+      <c r="I13" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1125,9 +1125,9 @@
         <v>2</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I14" s="6" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I14" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1168,7 +1168,7 @@
       <c r="H15" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="I15" s="8" t="inlineStr">
+      <c r="I15" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="I16" s="6" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
     </row>
@@ -1250,7 +1250,7 @@
       <c r="H17" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I17" s="6" t="inlineStr">
+      <c r="I17" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1291,7 +1291,7 @@
       <c r="H18" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I18" s="6" t="inlineStr">
+      <c r="I18" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1332,7 +1332,7 @@
       <c r="H19" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I19" s="8" t="inlineStr">
+      <c r="I19" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1373,7 +1373,7 @@
       <c r="H20" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I20" s="6" t="inlineStr">
+      <c r="I20" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1414,7 +1414,7 @@
       <c r="H21" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I21" s="6" t="inlineStr">
+      <c r="I21" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1455,7 +1455,7 @@
       <c r="H22" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I22" s="8" t="inlineStr">
+      <c r="I22" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1496,7 +1496,7 @@
       <c r="H23" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I23" s="6" t="inlineStr">
+      <c r="I23" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1537,7 +1537,7 @@
       <c r="H24" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I24" s="6" t="inlineStr">
+      <c r="I24" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1578,7 +1578,7 @@
       <c r="H25" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I25" s="6" t="inlineStr">
+      <c r="I25" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1619,7 +1619,7 @@
       <c r="H26" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I26" s="6" t="inlineStr">
+      <c r="I26" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1660,7 +1660,7 @@
       <c r="H27" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I27" s="8" t="inlineStr">
+      <c r="I27" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1701,7 +1701,7 @@
       <c r="H28" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I28" s="8" t="inlineStr">
+      <c r="I28" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="I29" s="6" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
     </row>
@@ -1783,7 +1783,7 @@
       <c r="H30" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I30" s="8" t="inlineStr">
+      <c r="I30" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="I31" s="6" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
     </row>
@@ -1865,7 +1865,7 @@
       <c r="H32" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I32" s="6" t="inlineStr">
+      <c r="I32" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1906,7 +1906,7 @@
       <c r="H33" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I33" s="6" t="inlineStr">
+      <c r="I33" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1947,7 +1947,7 @@
       <c r="H34" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="I34" s="8" t="inlineStr">
+      <c r="I34" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1986,9 +1986,9 @@
         <v>2</v>
       </c>
       <c r="H35" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="I35" s="6" t="inlineStr">
+        <v>7</v>
+      </c>
+      <c r="I35" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2029,7 +2029,7 @@
       <c r="H36" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I36" s="6" t="inlineStr">
+      <c r="I36" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2111,7 +2111,7 @@
       <c r="H38" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I38" s="6" t="inlineStr">
+      <c r="I38" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2191,9 +2191,9 @@
         <v>2</v>
       </c>
       <c r="H40" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="I40" s="6" t="inlineStr">
+        <v>7</v>
+      </c>
+      <c r="I40" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2234,7 +2234,7 @@
       <c r="H41" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I41" s="6" t="inlineStr">
+      <c r="I41" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="I42" s="6" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
     </row>
@@ -2316,7 +2316,7 @@
       <c r="H43" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I43" s="6" t="inlineStr">
+      <c r="I43" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2357,7 +2357,7 @@
       <c r="H44" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I44" s="6" t="inlineStr">
+      <c r="I44" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2398,7 +2398,7 @@
       <c r="H45" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I45" s="6" t="inlineStr">
+      <c r="I45" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2439,7 +2439,7 @@
       <c r="H46" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I46" s="6" t="inlineStr">
+      <c r="I46" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2480,7 +2480,7 @@
       <c r="H47" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I47" s="8" t="inlineStr">
+      <c r="I47" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -2521,7 +2521,7 @@
       <c r="H48" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="I48" s="8" t="inlineStr">
+      <c r="I48" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -2562,7 +2562,7 @@
       <c r="H49" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I49" s="6" t="inlineStr">
+      <c r="I49" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2644,7 +2644,7 @@
       <c r="H51" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I51" s="6" t="inlineStr">
+      <c r="I51" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2685,7 +2685,7 @@
       <c r="H52" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I52" s="6" t="inlineStr">
+      <c r="I52" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2726,7 +2726,7 @@
       <c r="H53" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I53" s="6" t="inlineStr">
+      <c r="I53" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2767,7 +2767,7 @@
       <c r="H54" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I54" s="6" t="inlineStr">
+      <c r="I54" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2808,7 +2808,7 @@
       <c r="H55" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I55" s="6" t="inlineStr">
+      <c r="I55" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2833,14 +2833,14 @@
           <t>Enviado</t>
         </is>
       </c>
-      <c r="E56" s="5" t="inlineStr">
-        <is>
-          <t>Ausente</t>
-        </is>
-      </c>
-      <c r="F56" s="5" t="inlineStr">
-        <is>
-          <t>Ausente</t>
+      <c r="E56" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F56" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="G56" s="3" t="n">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="I56" s="8" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -2888,9 +2888,9 @@
         <v>2</v>
       </c>
       <c r="H57" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="I57" s="6" t="inlineStr">
+        <v>7</v>
+      </c>
+      <c r="I57" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2931,7 +2931,7 @@
       <c r="H58" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I58" s="6" t="inlineStr">
+      <c r="I58" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2972,7 +2972,7 @@
       <c r="H59" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="I59" s="8" t="inlineStr">
+      <c r="I59" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -3095,7 +3095,7 @@
       <c r="H62" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I62" s="6" t="inlineStr">
+      <c r="I62" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -3136,7 +3136,7 @@
       <c r="H63" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I63" s="6" t="inlineStr">
+      <c r="I63" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -3177,7 +3177,7 @@
       <c r="H64" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I64" s="8" t="inlineStr">
+      <c r="I64" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -3218,7 +3218,7 @@
       <c r="H65" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I65" s="6" t="inlineStr">
+      <c r="I65" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -3259,7 +3259,7 @@
       <c r="H66" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I66" s="6" t="inlineStr">
+      <c r="I66" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -3300,7 +3300,7 @@
       <c r="H67" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I67" s="6" t="inlineStr">
+      <c r="I67" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -3341,7 +3341,7 @@
       <c r="H68" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I68" s="6" t="inlineStr">
+      <c r="I68" s="8" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -3382,7 +3382,7 @@
       <c r="H69" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I69" s="8" t="inlineStr">
+      <c r="I69" s="6" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>

</xml_diff>

<commit_message>
quebra de linha observações
</commit_message>
<xml_diff>
--- a/analise_engajamento.xlsx
+++ b/analise_engajamento.xlsx
@@ -70,8 +70,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFC107"/>
-        <bgColor rgb="00FFC107"/>
+        <fgColor rgb="00006400"/>
+        <bgColor rgb="00006400"/>
       </patternFill>
     </fill>
     <fill>
@@ -82,8 +82,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00006400"/>
-        <bgColor rgb="00006400"/>
+        <fgColor rgb="00FFC107"/>
+        <bgColor rgb="00FFC107"/>
       </patternFill>
     </fill>
     <fill>
@@ -532,7 +532,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,11 +633,11 @@
         <v>2</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I2" s="6" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -715,11 +715,11 @@
         <v>2</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I4" s="6" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -756,9 +756,9 @@
         <v>2</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I5" s="6" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I5" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -797,9 +797,9 @@
         <v>2</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I6" s="6" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I6" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -920,11 +920,11 @@
         <v>1</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I9" s="6" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -961,9 +961,9 @@
         <v>2</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I10" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I10" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1002,9 +1002,9 @@
         <v>2</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I11" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I11" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1045,7 +1045,7 @@
       <c r="H12" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I12" s="6" t="inlineStr">
+      <c r="I12" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1086,7 +1086,7 @@
       <c r="H13" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I13" s="8" t="inlineStr">
+      <c r="I13" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1127,7 +1127,7 @@
       <c r="H14" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="I14" s="8" t="inlineStr">
+      <c r="I14" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1166,9 +1166,9 @@
         <v>1</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="I15" s="6" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="I15" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1207,11 +1207,11 @@
         <v>2</v>
       </c>
       <c r="H16" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I16" s="6" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -1248,9 +1248,9 @@
         <v>2</v>
       </c>
       <c r="H17" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I17" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I17" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1289,9 +1289,9 @@
         <v>2</v>
       </c>
       <c r="H18" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I18" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I18" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1330,9 +1330,9 @@
         <v>2</v>
       </c>
       <c r="H19" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I19" s="6" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I19" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1371,9 +1371,9 @@
         <v>2</v>
       </c>
       <c r="H20" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I20" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I20" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1412,9 +1412,9 @@
         <v>2</v>
       </c>
       <c r="H21" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I21" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I21" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1453,9 +1453,9 @@
         <v>2</v>
       </c>
       <c r="H22" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="I22" s="6" t="inlineStr">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1494,9 +1494,9 @@
         <v>2</v>
       </c>
       <c r="H23" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I23" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I23" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1535,9 +1535,9 @@
         <v>2</v>
       </c>
       <c r="H24" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I24" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I24" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1576,9 +1576,9 @@
         <v>2</v>
       </c>
       <c r="H25" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I25" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I25" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1617,9 +1617,9 @@
         <v>2</v>
       </c>
       <c r="H26" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I26" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I26" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1658,9 +1658,9 @@
         <v>2</v>
       </c>
       <c r="H27" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I27" s="6" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I27" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1699,9 +1699,9 @@
         <v>2</v>
       </c>
       <c r="H28" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I28" s="6" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I28" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1740,11 +1740,11 @@
         <v>2</v>
       </c>
       <c r="H29" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I29" s="6" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -1781,9 +1781,9 @@
         <v>1</v>
       </c>
       <c r="H30" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="I30" s="6" t="inlineStr">
+        <v>7</v>
+      </c>
+      <c r="I30" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1822,11 +1822,11 @@
         <v>1</v>
       </c>
       <c r="H31" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I31" s="6" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -1863,9 +1863,9 @@
         <v>2</v>
       </c>
       <c r="H32" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I32" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I32" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1904,9 +1904,9 @@
         <v>2</v>
       </c>
       <c r="H33" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I33" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I33" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -1945,9 +1945,9 @@
         <v>1</v>
       </c>
       <c r="H34" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="I34" s="6" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="I34" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -1988,7 +1988,7 @@
       <c r="H35" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I35" s="8" t="inlineStr">
+      <c r="I35" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2027,9 +2027,9 @@
         <v>2</v>
       </c>
       <c r="H36" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I36" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I36" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2109,9 +2109,9 @@
         <v>2</v>
       </c>
       <c r="H38" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I38" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I38" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2150,11 +2150,11 @@
         <v>1</v>
       </c>
       <c r="H39" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="I39" s="7" t="inlineStr">
-        <is>
-          <t>Baixo</t>
+        <v>7</v>
+      </c>
+      <c r="I39" s="8" t="inlineStr">
+        <is>
+          <t>Médio</t>
         </is>
       </c>
     </row>
@@ -2191,9 +2191,9 @@
         <v>2</v>
       </c>
       <c r="H40" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I40" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I40" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2232,9 +2232,9 @@
         <v>2</v>
       </c>
       <c r="H41" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I41" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I41" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2273,11 +2273,11 @@
         <v>2</v>
       </c>
       <c r="H42" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I42" s="6" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -2293,7 +2293,7 @@
         </is>
       </c>
       <c r="C43" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" s="4" t="inlineStr">
         <is>
@@ -2305,20 +2305,20 @@
           <t>Enviado</t>
         </is>
       </c>
-      <c r="F43" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
+      <c r="F43" s="5" t="inlineStr">
+        <is>
+          <t>Ausente</t>
         </is>
       </c>
       <c r="G43" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H43" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I43" s="8" t="inlineStr">
-        <is>
-          <t>Alto</t>
+        <v>1</v>
+      </c>
+      <c r="I43" s="7" t="inlineStr">
+        <is>
+          <t>Baixo</t>
         </is>
       </c>
     </row>
@@ -2334,7 +2334,7 @@
         </is>
       </c>
       <c r="C44" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D44" s="4" t="inlineStr">
         <is>
@@ -2355,9 +2355,9 @@
         <v>2</v>
       </c>
       <c r="H44" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I44" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I44" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2375,7 +2375,7 @@
         </is>
       </c>
       <c r="C45" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D45" s="4" t="inlineStr">
         <is>
@@ -2396,9 +2396,9 @@
         <v>2</v>
       </c>
       <c r="H45" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I45" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I45" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2416,7 +2416,7 @@
         </is>
       </c>
       <c r="C46" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D46" s="4" t="inlineStr">
         <is>
@@ -2437,9 +2437,9 @@
         <v>2</v>
       </c>
       <c r="H46" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I46" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I46" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="C47" s="3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D47" s="4" t="inlineStr">
         <is>
@@ -2475,14 +2475,14 @@
         </is>
       </c>
       <c r="G47" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H47" s="3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I47" s="6" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -2498,7 +2498,7 @@
         </is>
       </c>
       <c r="C48" s="3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D48" s="4" t="inlineStr">
         <is>
@@ -2516,12 +2516,12 @@
         </is>
       </c>
       <c r="G48" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H48" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="I48" s="6" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="I48" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>
@@ -2539,7 +2539,7 @@
         </is>
       </c>
       <c r="C49" s="3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D49" s="4" t="inlineStr">
         <is>
@@ -2560,11 +2560,11 @@
         <v>2</v>
       </c>
       <c r="H49" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I49" s="8" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
     </row>
@@ -2580,7 +2580,7 @@
         </is>
       </c>
       <c r="C50" s="3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D50" s="4" t="inlineStr">
         <is>
@@ -2592,20 +2592,20 @@
           <t>Enviado</t>
         </is>
       </c>
-      <c r="F50" s="5" t="inlineStr">
-        <is>
-          <t>Ausente</t>
+      <c r="F50" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="G50" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H50" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="I50" s="7" t="inlineStr">
-        <is>
-          <t>Baixo</t>
+        <v>8</v>
+      </c>
+      <c r="I50" s="6" t="inlineStr">
+        <is>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -2617,11 +2617,11 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>Matelândia</t>
+          <t>Foz do Iguaçu</t>
         </is>
       </c>
       <c r="C51" s="3" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D51" s="4" t="inlineStr">
         <is>
@@ -2639,14 +2639,14 @@
         </is>
       </c>
       <c r="G51" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H51" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I51" s="8" t="inlineStr">
-        <is>
-          <t>Alto</t>
+        <v>3</v>
+      </c>
+      <c r="I51" s="7" t="inlineStr">
+        <is>
+          <t>Baixo</t>
         </is>
       </c>
     </row>
@@ -2658,7 +2658,7 @@
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>Medianeira</t>
+          <t>Matelândia</t>
         </is>
       </c>
       <c r="C52" s="3" t="n">
@@ -2683,9 +2683,9 @@
         <v>2</v>
       </c>
       <c r="H52" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I52" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I52" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2699,7 +2699,7 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>Santa Terezinha de Itaipu</t>
+          <t>Medianeira</t>
         </is>
       </c>
       <c r="C53" s="3" t="n">
@@ -2724,9 +2724,9 @@
         <v>2</v>
       </c>
       <c r="H53" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I53" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I53" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>São Miguel do Iguaçu</t>
+          <t>Santa Terezinha de Itaipu</t>
         </is>
       </c>
       <c r="C54" s="3" t="n">
@@ -2765,9 +2765,9 @@
         <v>2</v>
       </c>
       <c r="H54" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I54" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I54" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2781,50 +2781,50 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
+          <t>São Miguel do Iguaçu</t>
+        </is>
+      </c>
+      <c r="C55" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F55" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="G55" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H55" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="I55" s="6" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="11" t="inlineStr">
+        <is>
+          <t>Larissa</t>
+        </is>
+      </c>
+      <c r="B56" s="3" t="inlineStr">
+        <is>
           <t>Serranopolis do Iguaçu</t>
         </is>
       </c>
-      <c r="C55" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D55" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E55" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="F55" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="G55" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H55" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I55" s="8" t="inlineStr">
-        <is>
-          <t>Alto</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="12" t="inlineStr">
-        <is>
-          <t>Luana</t>
-        </is>
-      </c>
-      <c r="B56" s="3" t="inlineStr">
-        <is>
-          <t>Céu Azul</t>
-        </is>
-      </c>
       <c r="C56" s="3" t="n">
         <v>1</v>
       </c>
@@ -2847,9 +2847,9 @@
         <v>2</v>
       </c>
       <c r="H56" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I56" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I56" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2863,7 +2863,7 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>Diamante d'Oeste</t>
+          <t>Céu Azul</t>
         </is>
       </c>
       <c r="C57" s="3" t="n">
@@ -2888,9 +2888,9 @@
         <v>2</v>
       </c>
       <c r="H57" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I57" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I57" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>Entre Rios do Oeste</t>
+          <t>Diamante d'Oeste</t>
         </is>
       </c>
       <c r="C58" s="3" t="n">
@@ -2931,7 +2931,7 @@
       <c r="H58" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I58" s="8" t="inlineStr">
+      <c r="I58" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -2945,7 +2945,7 @@
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>Itaipulândia</t>
+          <t>Entre Rios do Oeste</t>
         </is>
       </c>
       <c r="C59" s="3" t="n">
@@ -2970,11 +2970,11 @@
         <v>2</v>
       </c>
       <c r="H59" s="3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I59" s="6" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>Marechal Candido Rondon</t>
+          <t>Itaipulândia</t>
         </is>
       </c>
       <c r="C60" s="3" t="n">
@@ -3008,14 +3008,14 @@
         </is>
       </c>
       <c r="G60" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H60" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="I60" s="7" t="inlineStr">
-        <is>
-          <t>Baixo</t>
+        <v>7</v>
+      </c>
+      <c r="I60" s="6" t="inlineStr">
+        <is>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -3031,7 +3031,7 @@
         </is>
       </c>
       <c r="C61" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="4" t="inlineStr">
         <is>
@@ -3049,10 +3049,10 @@
         </is>
       </c>
       <c r="G61" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I61" s="7" t="inlineStr">
         <is>
@@ -3068,11 +3068,11 @@
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>Missal</t>
+          <t>Marechal Candido Rondon</t>
         </is>
       </c>
       <c r="C62" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D62" s="4" t="inlineStr">
         <is>
@@ -3090,14 +3090,14 @@
         </is>
       </c>
       <c r="G62" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H62" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I62" s="8" t="inlineStr">
-        <is>
-          <t>Alto</t>
+        <v>2</v>
+      </c>
+      <c r="I62" s="7" t="inlineStr">
+        <is>
+          <t>Baixo</t>
         </is>
       </c>
     </row>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>Pato Bragado</t>
+          <t>Missal</t>
         </is>
       </c>
       <c r="C63" s="3" t="n">
@@ -3134,9 +3134,9 @@
         <v>2</v>
       </c>
       <c r="H63" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I63" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I63" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -3150,7 +3150,7 @@
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>Ramilândia</t>
+          <t>Pato Bragado</t>
         </is>
       </c>
       <c r="C64" s="3" t="n">
@@ -3161,25 +3161,25 @@
           <t>Enviado</t>
         </is>
       </c>
-      <c r="E64" s="5" t="inlineStr">
-        <is>
-          <t>Ausente</t>
-        </is>
-      </c>
-      <c r="F64" s="5" t="inlineStr">
-        <is>
-          <t>Ausente</t>
+      <c r="E64" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F64" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
         </is>
       </c>
       <c r="G64" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H64" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I64" s="6" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
     </row>
@@ -3191,7 +3191,7 @@
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>Santa Helena</t>
+          <t>Ramilândia</t>
         </is>
       </c>
       <c r="C65" s="3" t="n">
@@ -3202,25 +3202,25 @@
           <t>Enviado</t>
         </is>
       </c>
-      <c r="E65" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="F65" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
+      <c r="E65" s="5" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="F65" s="5" t="inlineStr">
+        <is>
+          <t>Ausente</t>
         </is>
       </c>
       <c r="G65" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H65" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I65" s="8" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
     </row>
@@ -3232,7 +3232,7 @@
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>Santa Tereza do Oeste</t>
+          <t>Santa Helena</t>
         </is>
       </c>
       <c r="C66" s="3" t="n">
@@ -3259,7 +3259,7 @@
       <c r="H66" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I66" s="8" t="inlineStr">
+      <c r="I66" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>São Jose das Palmeiras</t>
+          <t>Santa Tereza do Oeste</t>
         </is>
       </c>
       <c r="C67" s="3" t="n">
@@ -3298,9 +3298,9 @@
         <v>2</v>
       </c>
       <c r="H67" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I67" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I67" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>São Pedro do Iguaçu</t>
+          <t>São Jose das Palmeiras</t>
         </is>
       </c>
       <c r="C68" s="3" t="n">
@@ -3339,9 +3339,9 @@
         <v>2</v>
       </c>
       <c r="H68" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I68" s="8" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="I68" s="6" t="inlineStr">
         <is>
           <t>Alto</t>
         </is>
@@ -3355,34 +3355,75 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
+          <t>São Pedro do Iguaçu</t>
+        </is>
+      </c>
+      <c r="C69" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="E69" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F69" s="4" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="G69" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H69" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="I69" s="6" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="12" t="inlineStr">
+        <is>
+          <t>Luana</t>
+        </is>
+      </c>
+      <c r="B70" s="3" t="inlineStr">
+        <is>
           <t>Vera Cruz do Oeste</t>
         </is>
       </c>
-      <c r="C69" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D69" s="5" t="inlineStr">
+      <c r="C70" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" s="5" t="inlineStr">
         <is>
           <t>Ausente</t>
         </is>
       </c>
-      <c r="E69" s="5" t="inlineStr">
+      <c r="E70" s="5" t="inlineStr">
         <is>
           <t>Ausente</t>
         </is>
       </c>
-      <c r="F69" s="5" t="inlineStr">
+      <c r="F70" s="5" t="inlineStr">
         <is>
           <t>Ausente</t>
         </is>
       </c>
-      <c r="G69" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H69" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="I69" s="6" t="inlineStr">
+      <c r="G70" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H70" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="I70" s="8" t="inlineStr">
         <is>
           <t>Médio</t>
         </is>

</xml_diff>